<commit_message>
Rerunning ngrams + results
</commit_message>
<xml_diff>
--- a/data/ngram_stats/upos_bigrams.xlsx
+++ b/data/ngram_stats/upos_bigrams.xlsx
@@ -481,7 +481,7 @@
         <v>0.4549006474659522</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1784707871501033</v>
+        <v>0.187863986473793</v>
       </c>
     </row>
     <row r="3">
@@ -509,7 +509,7 @@
         <v>0.3907122125474436</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2348299830922412</v>
+        <v>0.2254367837685516</v>
       </c>
     </row>
     <row r="5">
@@ -579,7 +579,7 @@
         <v>1.311676713552132</v>
       </c>
       <c r="D9" t="n">
-        <v>0.8735675371031374</v>
+        <v>0.8453879391320683</v>
       </c>
     </row>
     <row r="10">
@@ -635,7 +635,7 @@
         <v>0.2539629381558384</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1408979898553447</v>
+        <v>0.1502911891790344</v>
       </c>
     </row>
     <row r="14">
@@ -677,7 +677,7 @@
         <v>1.024224157177942</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8078151418373097</v>
+        <v>0.826601540484689</v>
       </c>
     </row>
     <row r="17">
@@ -737,7 +737,7 @@
         <v>1.158182630051351</v>
       </c>
       <c r="D20" t="n">
-        <v>0.9768927296637234</v>
+        <v>0.9862859289874132</v>
       </c>
     </row>
     <row r="21">
@@ -779,7 +779,7 @@
         <v>0.3376869837017191</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4508735675371032</v>
+        <v>0.4602667668607928</v>
       </c>
     </row>
     <row r="24">
@@ -793,7 +793,7 @@
         <v>0.02511721366376423</v>
       </c>
       <c r="D24" t="n">
-        <v>0.1408979898553447</v>
+        <v>0.1502911891790344</v>
       </c>
     </row>
     <row r="25">
@@ -835,7 +835,7 @@
         <v>0.06418843491850859</v>
       </c>
       <c r="D27" t="n">
-        <v>0.1033251925605861</v>
+        <v>0.09393199323689649</v>
       </c>
     </row>
     <row r="28">
@@ -877,7 +877,7 @@
         <v>1.822393391382005</v>
       </c>
       <c r="D30" t="n">
-        <v>1.399586699229758</v>
+        <v>1.427766297200826</v>
       </c>
     </row>
     <row r="31">
@@ -891,7 +891,7 @@
         <v>0.05302522884572449</v>
       </c>
       <c r="D31" t="n">
-        <v>0.1033251925605861</v>
+        <v>0.1127183918842758</v>
       </c>
     </row>
     <row r="32">
@@ -905,7 +905,7 @@
         <v>0.3460593882563072</v>
       </c>
       <c r="D32" t="n">
-        <v>0.4884463648318617</v>
+        <v>0.5166259628029307</v>
       </c>
     </row>
     <row r="33">
@@ -937,7 +937,7 @@
         <v>1.576802857780754</v>
       </c>
       <c r="D34" t="n">
-        <v>1.268081908698103</v>
+        <v>1.315047905316551</v>
       </c>
     </row>
     <row r="35">
@@ -951,7 +951,7 @@
         <v>0.1367492743916053</v>
       </c>
       <c r="D35" t="n">
-        <v>0.1127183918842758</v>
+        <v>0.1033251925605861</v>
       </c>
     </row>
     <row r="36">
@@ -965,7 +965,7 @@
         <v>0.6670015628488503</v>
       </c>
       <c r="D36" t="n">
-        <v>0.9862859289874132</v>
+        <v>0.9956791283111027</v>
       </c>
     </row>
     <row r="37">
@@ -1021,7 +1021,7 @@
         <v>0.7367716008037508</v>
       </c>
       <c r="D40" t="n">
-        <v>0.8735675371031374</v>
+        <v>0.8641743377794476</v>
       </c>
     </row>
     <row r="41">
@@ -1035,7 +1035,7 @@
         <v>0.5665327081937932</v>
       </c>
       <c r="D41" t="n">
-        <v>1.906819462708999</v>
+        <v>1.87863986473793</v>
       </c>
     </row>
     <row r="42">
@@ -1063,7 +1063,7 @@
         <v>0.002790801518196026</v>
       </c>
       <c r="D43" t="n">
-        <v>0.0375727972947586</v>
+        <v>0.0187863986473793</v>
       </c>
     </row>
     <row r="44">
@@ -1109,7 +1109,7 @@
         <v>0.320942174592543</v>
       </c>
       <c r="D46" t="n">
-        <v>0.4414803682134135</v>
+        <v>0.4320871688897238</v>
       </c>
     </row>
     <row r="47">
@@ -1123,7 +1123,7 @@
         <v>0.2009377093101138</v>
       </c>
       <c r="D47" t="n">
-        <v>0.159684388502724</v>
+        <v>0.1690775878264137</v>
       </c>
     </row>
     <row r="48">
@@ -1207,7 +1207,7 @@
         <v>0.1841929002009377</v>
       </c>
       <c r="D53" t="n">
-        <v>0.1127183918842758</v>
+        <v>0.1221115912079654</v>
       </c>
     </row>
     <row r="54">
@@ -1235,7 +1235,7 @@
         <v>0.04186202277294039</v>
       </c>
       <c r="D55" t="n">
-        <v>0.0375727972947586</v>
+        <v>0.04696599661844825</v>
       </c>
     </row>
     <row r="56">
@@ -1249,7 +1249,7 @@
         <v>0.4465282429113642</v>
       </c>
       <c r="D56" t="n">
-        <v>0.1972571857974826</v>
+        <v>0.187863986473793</v>
       </c>
     </row>
     <row r="57">
@@ -1277,7 +1277,7 @@
         <v>0.7339807992855548</v>
       </c>
       <c r="D58" t="n">
-        <v>0.7702423445425512</v>
+        <v>0.7608491452188616</v>
       </c>
     </row>
     <row r="59">
@@ -1295,7 +1295,7 @@
         <v>0.5944407233757536</v>
       </c>
       <c r="D59" t="n">
-        <v>0.347548374976517</v>
+        <v>0.3569415743002066</v>
       </c>
     </row>
     <row r="60">
@@ -1323,7 +1323,7 @@
         <v>0.1786112971645457</v>
       </c>
       <c r="D61" t="n">
-        <v>0.2254367837685516</v>
+        <v>0.2442231824159309</v>
       </c>
     </row>
     <row r="62">
@@ -1337,7 +1337,7 @@
         <v>0.1758204956463496</v>
       </c>
       <c r="D62" t="n">
-        <v>0.2724027803869998</v>
+        <v>0.2630095810633102</v>
       </c>
     </row>
     <row r="63">
@@ -1379,7 +1379,7 @@
         <v>0.2902433578923867</v>
       </c>
       <c r="D65" t="n">
-        <v>0.5166259628029307</v>
+        <v>0.5260191621266204</v>
       </c>
     </row>
     <row r="66">
@@ -1407,7 +1407,7 @@
         <v>0.1423308774279973</v>
       </c>
       <c r="D67" t="n">
-        <v>0.09393199323689649</v>
+        <v>0.1033251925605861</v>
       </c>
     </row>
     <row r="68">
@@ -1463,7 +1463,7 @@
         <v>0.0111632060727841</v>
       </c>
       <c r="D71" t="n">
-        <v>0.02817959797106895</v>
+        <v>0.0187863986473793</v>
       </c>
     </row>
     <row r="72">
@@ -1495,7 +1495,7 @@
         <v>0.4353650368385801</v>
       </c>
       <c r="D73" t="n">
-        <v>0.5072327634792411</v>
+        <v>0.4978395641555514</v>
       </c>
     </row>
     <row r="74">
@@ -1537,7 +1537,7 @@
         <v>0.01674480910917615</v>
       </c>
       <c r="D76" t="n">
-        <v>0.0751455945895172</v>
+        <v>0.06575239526582755</v>
       </c>
     </row>
     <row r="77">
@@ -1551,7 +1551,7 @@
         <v>0.103259656173253</v>
       </c>
       <c r="D77" t="n">
-        <v>0.1315047905316551</v>
+        <v>0.1221115912079654</v>
       </c>
     </row>
     <row r="78">
@@ -1565,7 +1565,7 @@
         <v>0.04465282429113641</v>
       </c>
       <c r="D78" t="n">
-        <v>0.1315047905316551</v>
+        <v>0.1408979898553447</v>
       </c>
     </row>
     <row r="79">
@@ -1579,7 +1579,7 @@
         <v>0.9153828979682964</v>
       </c>
       <c r="D79" t="n">
-        <v>1.465339094495585</v>
+        <v>1.493518692466654</v>
       </c>
     </row>
     <row r="80">
@@ -1607,7 +1607,7 @@
         <v>0.2037285108283099</v>
       </c>
       <c r="D81" t="n">
-        <v>0.1502911891790344</v>
+        <v>0.1690775878264137</v>
       </c>
     </row>
     <row r="82">
@@ -1621,7 +1621,7 @@
         <v>0.1479124804643894</v>
       </c>
       <c r="D82" t="n">
-        <v>0.2066503851211723</v>
+        <v>0.1972571857974826</v>
       </c>
     </row>
     <row r="83">
@@ -1663,7 +1663,7 @@
         <v>0.03348961821835231</v>
       </c>
       <c r="D85" t="n">
-        <v>0.1315047905316551</v>
+        <v>0.1221115912079654</v>
       </c>
     </row>
     <row r="86">
@@ -1709,7 +1709,7 @@
         <v>0.2260549229738781</v>
       </c>
       <c r="D88" t="n">
-        <v>0.2442231824159309</v>
+        <v>0.2536163817396205</v>
       </c>
     </row>
     <row r="89">
@@ -1765,7 +1765,7 @@
         <v>0.02232641214556821</v>
       </c>
       <c r="D92" t="n">
-        <v>0.09393199323689649</v>
+        <v>0.1033251925605861</v>
       </c>
     </row>
     <row r="93">
@@ -1793,7 +1793,7 @@
         <v>1.353538736325073</v>
       </c>
       <c r="D94" t="n">
-        <v>2.057110651888033</v>
+        <v>2.047717452564344</v>
       </c>
     </row>
     <row r="95">
@@ -1863,7 +1863,7 @@
         <v>0.07814244250948872</v>
       </c>
       <c r="D99" t="n">
-        <v>0.09393199323689649</v>
+        <v>0.1033251925605861</v>
       </c>
     </row>
     <row r="100">
@@ -1877,7 +1877,7 @@
         <v>0.03907122125474436</v>
       </c>
       <c r="D100" t="n">
-        <v>0.02817959797106895</v>
+        <v>0.0375727972947586</v>
       </c>
     </row>
     <row r="101">
@@ -1891,7 +1891,7 @@
         <v>0.3711766019200715</v>
       </c>
       <c r="D101" t="n">
-        <v>0.5823783580687583</v>
+        <v>0.6105579560398272</v>
       </c>
     </row>
     <row r="102">
@@ -1983,7 +1983,7 @@
         <v>3.379660638535388</v>
       </c>
       <c r="D107" t="n">
-        <v>2.874318993049032</v>
+        <v>2.911891790343791</v>
       </c>
     </row>
     <row r="108">
@@ -1997,7 +1997,7 @@
         <v>3.00569323509712</v>
       </c>
       <c r="D108" t="n">
-        <v>3.015216982904377</v>
+        <v>3.024610182228067</v>
       </c>
     </row>
     <row r="109">
@@ -2025,7 +2025,7 @@
         <v>0.3572225943290913</v>
       </c>
       <c r="D110" t="n">
-        <v>0.3663347736238963</v>
+        <v>0.3851211722712756</v>
       </c>
     </row>
     <row r="111">
@@ -2067,7 +2067,7 @@
         <v>3.87642330877428</v>
       </c>
       <c r="D113" t="n">
-        <v>2.874318993049032</v>
+        <v>2.864925793725343</v>
       </c>
     </row>
     <row r="114">
@@ -2123,7 +2123,7 @@
         <v>0.7311899977673588</v>
       </c>
       <c r="D117" t="n">
-        <v>2.122863047153861</v>
+        <v>2.094683449182792</v>
       </c>
     </row>
     <row r="118">
@@ -2137,7 +2137,7 @@
         <v>6.943514177271711</v>
       </c>
       <c r="D118" t="n">
-        <v>4.743565658463273</v>
+        <v>4.724779259815894</v>
       </c>
     </row>
     <row r="119">
@@ -2165,7 +2165,7 @@
         <v>2.550792587631168</v>
       </c>
       <c r="D120" t="n">
-        <v>2.705241405222619</v>
+        <v>2.66766860792786</v>
       </c>
     </row>
     <row r="121">
@@ -2267,7 +2267,7 @@
         <v>0.4018754186202277</v>
       </c>
       <c r="D127" t="n">
-        <v>0.7044899492767236</v>
+        <v>0.7138831486004132</v>
       </c>
     </row>
     <row r="128">
@@ -2383,7 +2383,7 @@
         <v>0.2511721366376423</v>
       </c>
       <c r="D135" t="n">
-        <v>0.4039075709186549</v>
+        <v>0.4133007702423445</v>
       </c>
     </row>
     <row r="136">
@@ -2397,7 +2397,7 @@
         <v>0.2232641214556821</v>
       </c>
       <c r="D136" t="n">
-        <v>0.1127183918842758</v>
+        <v>0.1033251925605861</v>
       </c>
     </row>
     <row r="137">
@@ -2411,7 +2411,7 @@
         <v>0.1758204956463496</v>
       </c>
       <c r="D137" t="n">
-        <v>0.04696599661844825</v>
+        <v>0.0563591959421379</v>
       </c>
     </row>
     <row r="138">
@@ -2481,7 +2481,7 @@
         <v>0.1311676713552132</v>
       </c>
       <c r="D142" t="n">
-        <v>0.09393199323689649</v>
+        <v>0.08453879391320684</v>
       </c>
     </row>
     <row r="143">
@@ -2551,7 +2551,7 @@
         <v>1.096784996651038</v>
       </c>
       <c r="D147" t="n">
-        <v>0.375727972947586</v>
+        <v>0.3851211722712756</v>
       </c>
     </row>
     <row r="148">
@@ -2583,7 +2583,7 @@
         <v>0.3125697700379549</v>
       </c>
       <c r="D149" t="n">
-        <v>0.3005823783580688</v>
+        <v>0.2911891790343791</v>
       </c>
     </row>
     <row r="150">
@@ -2611,7 +2611,7 @@
         <v>0.2344273275284662</v>
       </c>
       <c r="D151" t="n">
-        <v>0.2160435844448619</v>
+        <v>0.2348299830922412</v>
       </c>
     </row>
     <row r="152">
@@ -2625,7 +2625,7 @@
         <v>0.05023442732752846</v>
       </c>
       <c r="D152" t="n">
-        <v>0.1315047905316551</v>
+        <v>0.1408979898553447</v>
       </c>
     </row>
     <row r="153">
@@ -2695,7 +2695,7 @@
         <v>0.2930341594105828</v>
       </c>
       <c r="D157" t="n">
-        <v>0.1221115912079654</v>
+        <v>0.1033251925605861</v>
       </c>
     </row>
     <row r="158">
@@ -2709,7 +2709,7 @@
         <v>0.2734985487832106</v>
       </c>
       <c r="D158" t="n">
-        <v>0.4414803682134135</v>
+        <v>0.4320871688897238</v>
       </c>
     </row>
     <row r="159">
@@ -2751,7 +2751,7 @@
         <v>0.04186202277294039</v>
       </c>
       <c r="D161" t="n">
-        <v>0.0563591959421379</v>
+        <v>0.04696599661844825</v>
       </c>
     </row>
     <row r="162">
@@ -2765,7 +2765,7 @@
         <v>0.8763116767135521</v>
       </c>
       <c r="D162" t="n">
-        <v>1.089611121547999</v>
+        <v>1.06143152357693</v>
       </c>
     </row>
     <row r="163">
@@ -2825,7 +2825,7 @@
         <v>0.212100915382898</v>
       </c>
       <c r="D166" t="n">
-        <v>0.9956791283111027</v>
+        <v>0.9768927296637234</v>
       </c>
     </row>
     <row r="167">
@@ -2881,7 +2881,7 @@
         <v>0.005581603036392052</v>
       </c>
       <c r="D170" t="n">
-        <v>0.06575239526582755</v>
+        <v>0.0563591959421379</v>
       </c>
     </row>
     <row r="171">
@@ -2895,7 +2895,7 @@
         <v>0.06977003795490065</v>
       </c>
       <c r="D171" t="n">
-        <v>0.4039075709186549</v>
+        <v>0.4133007702423445</v>
       </c>
     </row>
     <row r="172">
@@ -2979,7 +2979,7 @@
         <v>0.01395400759098013</v>
       </c>
       <c r="D177" t="n">
-        <v>0.0751455945895172</v>
+        <v>0.06575239526582755</v>
       </c>
     </row>
     <row r="178">
@@ -3081,7 +3081,7 @@
         <v>0.212100915382898</v>
       </c>
       <c r="D184" t="n">
-        <v>0.1502911891790344</v>
+        <v>0.1408979898553447</v>
       </c>
     </row>
     <row r="185">
@@ -3095,7 +3095,7 @@
         <v>0.7451440053583389</v>
       </c>
       <c r="D185" t="n">
-        <v>1.221115912079654</v>
+        <v>1.230509111403344</v>
       </c>
     </row>
     <row r="186">
@@ -3109,7 +3109,7 @@
         <v>0.4632730520205403</v>
       </c>
       <c r="D186" t="n">
-        <v>0.2911891790343791</v>
+        <v>0.3005823783580688</v>
       </c>
     </row>
     <row r="187">
@@ -3165,7 +3165,7 @@
         <v>0.3962938155838357</v>
       </c>
       <c r="D190" t="n">
-        <v>0.3381551756528274</v>
+        <v>0.3287619763291377</v>
       </c>
     </row>
     <row r="191">
@@ -3263,7 +3263,7 @@
         <v>0.1758204956463496</v>
       </c>
       <c r="D197" t="n">
-        <v>0.1408979898553447</v>
+        <v>0.1221115912079654</v>
       </c>
     </row>
     <row r="198">
@@ -3337,7 +3337,7 @@
         <v>0.002790801518196026</v>
       </c>
       <c r="D202" t="n">
-        <v>0.04696599661844825</v>
+        <v>0.0375727972947586</v>
       </c>
     </row>
     <row r="203">
@@ -3351,7 +3351,7 @@
         <v>0.07256083947309667</v>
       </c>
       <c r="D203" t="n">
-        <v>0.08453879391320684</v>
+        <v>0.09393199323689649</v>
       </c>
     </row>
     <row r="204">
@@ -3365,7 +3365,7 @@
         <v>0.3600133958472873</v>
       </c>
       <c r="D204" t="n">
-        <v>0.4320871688897238</v>
+        <v>0.4226939695660342</v>
       </c>
     </row>
     <row r="205">
@@ -3393,7 +3393,7 @@
         <v>0.1674480910917616</v>
       </c>
       <c r="D206" t="n">
-        <v>0.0751455945895172</v>
+        <v>0.08453879391320684</v>
       </c>
     </row>
     <row r="207">
@@ -3407,7 +3407,7 @@
         <v>0.1674480910917616</v>
       </c>
       <c r="D207" t="n">
-        <v>0.2817959797106894</v>
+        <v>0.2724027803869998</v>
       </c>
     </row>
     <row r="208">
@@ -3463,7 +3463,7 @@
         <v>0.4800178611297164</v>
       </c>
       <c r="D211" t="n">
-        <v>0.347548374976517</v>
+        <v>0.3381551756528274</v>
       </c>
     </row>
     <row r="212">
@@ -3527,7 +3527,7 @@
         <v>0.5693235097119892</v>
       </c>
       <c r="D215" t="n">
-        <v>0.4414803682134135</v>
+        <v>0.4320871688897238</v>
       </c>
     </row>
     <row r="216">
@@ -3541,7 +3541,7 @@
         <v>1.970305871846394</v>
       </c>
       <c r="D216" t="n">
-        <v>1.850460266766861</v>
+        <v>1.841067067443171</v>
       </c>
     </row>
     <row r="217">
@@ -3555,7 +3555,7 @@
         <v>0.3907122125474436</v>
       </c>
       <c r="D217" t="n">
-        <v>0.4414803682134135</v>
+        <v>0.4226939695660342</v>
       </c>
     </row>
     <row r="218">
@@ -3569,7 +3569,7 @@
         <v>0.759098012949319</v>
       </c>
       <c r="D218" t="n">
-        <v>0.53541236145031</v>
+        <v>0.5541987600976892</v>
       </c>
     </row>
     <row r="219">
@@ -3597,7 +3597,7 @@
         <v>0.320942174592543</v>
       </c>
       <c r="D220" t="n">
-        <v>0.2911891790343791</v>
+        <v>0.3099755776817584</v>
       </c>
     </row>
     <row r="221">
@@ -3611,7 +3611,7 @@
         <v>1.791694574681848</v>
       </c>
       <c r="D221" t="n">
-        <v>2.179222243095999</v>
+        <v>2.151042645124929</v>
       </c>
     </row>
     <row r="222">
@@ -3625,7 +3625,7 @@
         <v>0.0753516409912927</v>
       </c>
       <c r="D222" t="n">
-        <v>0.2066503851211723</v>
+        <v>0.2160435844448619</v>
       </c>
     </row>
     <row r="223">
@@ -3639,7 +3639,7 @@
         <v>0.3153605715561509</v>
       </c>
       <c r="D223" t="n">
-        <v>0.2911891790343791</v>
+        <v>0.3005823783580688</v>
       </c>
     </row>
     <row r="224">
@@ -3653,7 +3653,7 @@
         <v>1.855883009600357</v>
       </c>
       <c r="D224" t="n">
-        <v>1.841067067443171</v>
+        <v>1.831673868119482</v>
       </c>
     </row>
     <row r="225">
@@ -3667,7 +3667,7 @@
         <v>0.1618664880553695</v>
       </c>
       <c r="D225" t="n">
-        <v>0.1408979898553447</v>
+        <v>0.1502911891790344</v>
       </c>
     </row>
     <row r="226">
@@ -3723,7 +3723,7 @@
         <v>0.02790801518196026</v>
       </c>
       <c r="D229" t="n">
-        <v>0.0563591959421379</v>
+        <v>0.04696599661844825</v>
       </c>
     </row>
     <row r="230">
@@ -3825,7 +3825,7 @@
         <v>0.644675150703282</v>
       </c>
       <c r="D236" t="n">
-        <v>0.4602667668607928</v>
+        <v>0.4320871688897238</v>
       </c>
     </row>
     <row r="237">
@@ -3853,7 +3853,7 @@
         <v>0.04744362580933244</v>
       </c>
       <c r="D238" t="n">
-        <v>0.1033251925605861</v>
+        <v>0.1127183918842758</v>
       </c>
     </row>
     <row r="239">
@@ -3885,7 +3885,7 @@
         <v>0</v>
       </c>
       <c r="D240" t="n">
-        <v>0.0375727972947586</v>
+        <v>0.02817959797106895</v>
       </c>
     </row>
     <row r="241">

</xml_diff>